<commit_message>
Method up to cover amount slider component
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
+++ b/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE988DA8-AFB8-4348-9D49-2F4A9852423F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEECF40-05B2-4D7E-A5EB-89D9E8042F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="340" windowWidth="14400" windowHeight="7360" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
   </bookViews>
   <sheets>
     <sheet name="PolicyHolder_Details" sheetId="1" r:id="rId1"/>
-    <sheet name="PLA" sheetId="5" r:id="rId2"/>
-    <sheet name="Affordability_Check" sheetId="8" r:id="rId3"/>
-    <sheet name="Extended" sheetId="7" r:id="rId4"/>
-    <sheet name="Parent" sheetId="11" r:id="rId5"/>
-    <sheet name="Spouse" sheetId="6" r:id="rId6"/>
-    <sheet name="Beneficiaries" sheetId="9" r:id="rId7"/>
-    <sheet name="PolicyPayer" sheetId="10" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="PLA" sheetId="5" r:id="rId3"/>
+    <sheet name="Affordability_Check" sheetId="8" r:id="rId4"/>
+    <sheet name="Extended" sheetId="7" r:id="rId5"/>
+    <sheet name="Parent" sheetId="11" r:id="rId6"/>
+    <sheet name="Spouse" sheetId="6" r:id="rId7"/>
+    <sheet name="Beneficiaries" sheetId="9" r:id="rId8"/>
     <sheet name="Child" sheetId="12" r:id="rId9"/>
+    <sheet name="PolicyPayer" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="60">
   <si>
     <t>Town</t>
   </si>
@@ -201,13 +202,34 @@
   </si>
   <si>
     <t>Cousin</t>
+  </si>
+  <si>
+    <t>Cover Amount</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Extended</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,16 +258,60 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -279,6 +345,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -288,7 +380,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -311,6 +403,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -319,6 +436,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9966FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -629,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42906E6D-7A8E-4EC7-BEBD-C72FF8B2CEAE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -749,7 +871,427 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC2C190-2299-448D-81E7-FE582936E6E6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2">
+        <v>830678899</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="10">
+        <v>62429363625</v>
+      </c>
+      <c r="G2" s="2">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1A9CEFBF-6668-43EE-8C58-295655E6BCFD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A88081-1358-4BE1-BD13-46027B97D51F}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>7500</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7500</v>
+      </c>
+      <c r="D4" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>7500</v>
+      </c>
+      <c r="F4" s="3">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7500</v>
+      </c>
+      <c r="H4" s="15">
+        <v>14.2857</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7500</v>
+      </c>
+      <c r="J4" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="3">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="15">
+        <v>28.571400000000001</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="J5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>15000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>37.5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>15000</v>
+      </c>
+      <c r="D6" s="3">
+        <v>37.5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15000</v>
+      </c>
+      <c r="F6" s="3">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3">
+        <v>15000</v>
+      </c>
+      <c r="H6" s="15">
+        <v>42.857100000000003</v>
+      </c>
+      <c r="I6" s="3">
+        <v>15000</v>
+      </c>
+      <c r="J6" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>80</v>
+      </c>
+      <c r="G7" s="3">
+        <v>20000</v>
+      </c>
+      <c r="H7" s="15">
+        <v>57.142899999999997</v>
+      </c>
+      <c r="I7" s="3">
+        <v>20000</v>
+      </c>
+      <c r="J7" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>30000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>30000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>100</v>
+      </c>
+      <c r="G8" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H8" s="15">
+        <v>71.428600000000003</v>
+      </c>
+      <c r="I8" s="3">
+        <v>30000</v>
+      </c>
+      <c r="J8" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>40000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3">
+        <v>40000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>75</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>40000</v>
+      </c>
+      <c r="H9" s="14">
+        <v>85.714299999999994</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>50000</v>
+      </c>
+      <c r="H10" s="13">
+        <v>100</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>60000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>100</v>
+      </c>
+      <c r="C11" s="3">
+        <v>60000</v>
+      </c>
+      <c r="D11" s="3">
+        <v>100</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E14" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786073B4-85CC-4556-90E2-B38B107A54B7}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -859,7 +1401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C580E6-39BE-4917-B92D-9C5DAD8C2402}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K2"/>
@@ -954,7 +1496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB677AF7-CD04-4859-B2D3-DBB348803FA9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1022,7 +1564,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A25D57-60AB-4959-A648-53F314C54D9C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1083,7 +1625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44766631-B11A-4479-8024-A9637BA1BEB4}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1146,7 +1688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99D9670-810C-4DE3-B59B-B8F4007A7BBA}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1208,78 +1750,6 @@
       <c r="G7" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC2C190-2299-448D-81E7-FE582936E6E6}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2">
-        <v>830678899</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="10">
-        <v>62429363625</v>
-      </c>
-      <c r="G2" s="2">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1A9CEFBF-6668-43EE-8C58-295655E6BCFD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Code functionality  up to Payment Details
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
+++ b/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEECF40-05B2-4D7E-A5EB-89D9E8042F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A5DD43-8129-48F8-974A-DB17C9B5D4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="10" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
   </bookViews>
   <sheets>
     <sheet name="PolicyHolder_Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="Scroler" sheetId="13" r:id="rId2"/>
     <sheet name="PLA" sheetId="5" r:id="rId3"/>
     <sheet name="Affordability_Check" sheetId="8" r:id="rId4"/>
     <sheet name="Extended" sheetId="7" r:id="rId5"/>
@@ -23,6 +23,7 @@
     <sheet name="Beneficiaries" sheetId="9" r:id="rId8"/>
     <sheet name="Child" sheetId="12" r:id="rId9"/>
     <sheet name="PolicyPayer" sheetId="10" r:id="rId10"/>
+    <sheet name="BankDetails" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="76">
   <si>
     <t>Town</t>
   </si>
@@ -204,12 +205,6 @@
     <t>Cousin</t>
   </si>
   <si>
-    <t>Cover Amount</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
     <t>Self</t>
   </si>
   <si>
@@ -223,6 +218,60 @@
   </si>
   <si>
     <t>Extended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PercentagePayout </t>
+  </si>
+  <si>
+    <t>CoverAmountS</t>
+  </si>
+  <si>
+    <t>CoverAmountSP</t>
+  </si>
+  <si>
+    <t>CoverAmountP</t>
+  </si>
+  <si>
+    <t>CoverAmountC</t>
+  </si>
+  <si>
+    <t>CoverAmountE</t>
+  </si>
+  <si>
+    <t>widthS</t>
+  </si>
+  <si>
+    <t>widthSP</t>
+  </si>
+  <si>
+    <t>widthP</t>
+  </si>
+  <si>
+    <t>widthC</t>
+  </si>
+  <si>
+    <t>widthE</t>
+  </si>
+  <si>
+    <t>widthPP</t>
+  </si>
+  <si>
+    <t>Beneficiary</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>SalaryPaydate</t>
+  </si>
+  <si>
+    <t>FIRST NATIONAL BANK</t>
+  </si>
+  <si>
+    <t>debitOrderday</t>
   </si>
 </sst>
 </file>
@@ -311,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -371,6 +420,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -380,7 +451,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -413,12 +484,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -428,6 +493,21 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -943,79 +1023,134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5742EF1-81B6-4D29-8062-C3F3570B2BE5}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A88081-1358-4BE1-BD13-46027B97D51F}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="16" t="s">
+      <c r="F1" s="24"/>
+      <c r="G1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="16" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="16" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="22"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L2" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>5000</v>
       </c>
@@ -1046,8 +1181,14 @@
       <c r="J3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="2">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>7500</v>
       </c>
@@ -1079,7 +1220,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>10000</v>
       </c>
@@ -1111,7 +1252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>15000</v>
       </c>
@@ -1143,7 +1284,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>20000</v>
       </c>
@@ -1175,7 +1316,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>30000</v>
       </c>
@@ -1207,7 +1348,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>40000</v>
       </c>
@@ -1231,7 +1372,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>50000</v>
       </c>
@@ -1255,7 +1396,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>60000</v>
       </c>
@@ -1275,11 +1416,12 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E14" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>

</xml_diff>

<commit_message>
Push man Pusha man
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
+++ b/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE131A91-8855-4000-8033-B9DFCCDE087B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737CA5AC-9B01-4570-91F5-A3CE72395CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="7" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
   </bookViews>
   <sheets>
     <sheet name="PolicyHolder_Details" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,14 @@
     <sheet name="Cover_Coordinates" sheetId="13" r:id="rId4"/>
     <sheet name="PLA" sheetId="5" r:id="rId5"/>
     <sheet name="Affordability_Check" sheetId="8" r:id="rId6"/>
-    <sheet name="Extended" sheetId="7" r:id="rId7"/>
-    <sheet name="Parent" sheetId="11" r:id="rId8"/>
-    <sheet name="Spouse" sheetId="6" r:id="rId9"/>
-    <sheet name="Beneficiaries" sheetId="9" r:id="rId10"/>
-    <sheet name="Child" sheetId="12" r:id="rId11"/>
-    <sheet name="PolicyPayer" sheetId="10" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId7"/>
+    <sheet name="Scenarios" sheetId="17" r:id="rId8"/>
+    <sheet name="Extended" sheetId="7" r:id="rId9"/>
+    <sheet name="Parent" sheetId="11" r:id="rId10"/>
+    <sheet name="Spouse" sheetId="6" r:id="rId11"/>
+    <sheet name="Beneficiaries" sheetId="9" r:id="rId12"/>
+    <sheet name="Child" sheetId="12" r:id="rId13"/>
+    <sheet name="PolicyPayer" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="102">
   <si>
     <t>Town</t>
   </si>
@@ -197,9 +199,6 @@
     <t>LindoKuhle</t>
   </si>
   <si>
-    <t>SpouseMax1</t>
-  </si>
-  <si>
     <t>Extended_RelationshipType</t>
   </si>
   <si>
@@ -237,13 +236,143 @@
   </si>
   <si>
     <t>Scenaro_id</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Scenario detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expecteced Result </t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>Test__Date</t>
+  </si>
+  <si>
+    <t>Test Passed</t>
+  </si>
+  <si>
+    <t>Test Failed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test Total</t>
+    </r>
+  </si>
+  <si>
+    <t>New Business</t>
+  </si>
+  <si>
+    <t>Validations</t>
+  </si>
+  <si>
+    <t>Maximum Validation for spouse</t>
+  </si>
+  <si>
+    <t>Maximum Validation for Child</t>
+  </si>
+  <si>
+    <t>Maximum Validation for Parent</t>
+  </si>
+  <si>
+    <t>Maximum Validation for Extended</t>
+  </si>
+  <si>
+    <t>Maximum Validation for self</t>
+  </si>
+  <si>
+    <t>Minimum Validation for self</t>
+  </si>
+  <si>
+    <t>Minimum Validation for spouse</t>
+  </si>
+  <si>
+    <t>Maximum Validation for spouser</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>MaxSpouse</t>
+  </si>
+  <si>
+    <t>MaxChild</t>
+  </si>
+  <si>
+    <t>MaxParent</t>
+  </si>
+  <si>
+    <t>MaxExtended</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>Minspouse</t>
+  </si>
+  <si>
+    <t>Maxspouse</t>
+  </si>
+  <si>
+    <t>Maxsel</t>
+  </si>
+  <si>
+    <t>Minsel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +427,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +503,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA082F6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -385,6 +576,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -394,7 +644,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -442,13 +692,439 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{501A4514-B1BB-400C-AFA1-8FE92D854DF2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFA082F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -464,6 +1140,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77094FBE-62A7-4D62-9AD5-A2591B43D462}" name="Table2" displayName="Table2" ref="A1:J9" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:J9" xr:uid="{77094FBE-62A7-4D62-9AD5-A2591B43D462}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{8ECCF095-A47A-4446-88DE-C20C9EA98F17}" name="Scenario" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6F04CA4E-DCDF-4D0E-864E-A4EC9DCC22FA}" name="Product" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{90CFC39C-5F10-4E1C-A1C9-7C8B4689C428}" name="Functionality" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{7C56597E-D0E3-4A56-AB5D-05FE23C6E903}" name="Action" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{A6197CED-E60A-4FA0-B975-C7AAB97218D2}" name="Functions" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{CD1BEAF3-C27B-4209-B9B1-E5180FA9BCCB}" name="Scenario detail" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{75B480A5-EDCD-4306-BA1C-18ECE9AAAA09}" name="Expecteced Result " dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{B7BB90DE-DDCC-4FBC-8023-957CDA7ABAC9}" name="Comment" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{38E0EF8D-3901-4056-AA3F-B5BA1F059947}" name="Test Result" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{20682D0F-D730-43CC-A849-D092705CEA7C}" name="Test__Date" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -886,6 +1581,130 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A25D57-60AB-4959-A648-53F314C54D9C}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9">
+        <v>36202</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44766631-B11A-4479-8024-A9637BA1BEB4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9">
+        <v>36202</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99D9670-810C-4DE3-B59B-B8F4007A7BBA}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -951,7 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99637A6-F889-4564-89B2-AF62D5E8EE61}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1024,7 +1843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC2C190-2299-448D-81E7-FE582936E6E6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1111,15 +1930,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>60000</v>
@@ -1127,7 +1946,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>15000</v>
@@ -1135,7 +1954,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>7500</v>
@@ -1143,7 +1962,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>10000</v>
@@ -1151,7 +1970,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>20000</v>
@@ -1198,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1209,7 +2028,7 @@
         <v>12.5</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1220,7 +2039,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1231,7 +2050,7 @@
         <v>37.5</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1242,7 +2061,7 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1302,56 +2121,56 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="C2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="E2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="G2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="I2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1743,7 +2562,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1759,7 +2578,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -1840,11 +2659,290 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8670DEE1-CE9B-417F-9985-01ED7EF35F61}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED677DD-E8AF-421A-8C90-EED6078DC1A9}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A2" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="33"/>
+    </row>
+    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="33"/>
+    </row>
+    <row r="7" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="33"/>
+    </row>
+    <row r="8" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A8" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="33"/>
+    </row>
+    <row r="9" spans="1:14" ht="24" x14ac:dyDescent="0.35">
+      <c r="A9" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="27">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB677AF7-CD04-4859-B2D3-DBB348803FA9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1876,7 +2974,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1899,131 +2997,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A25D57-60AB-4959-A648-53F314C54D9C}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="9">
-        <v>36202</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44766631-B11A-4479-8024-A9637BA1BEB4}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="9">
-        <v>36202</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Min Max age complete\
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
+++ b/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA55879-0CB3-4DDD-B6F0-1DA4C083F38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA4A225-B4D8-49D1-80AC-2A9ADB120335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="7" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="7" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
   </bookViews>
   <sheets>
     <sheet name="PolicyHolder_Details" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="96">
   <si>
     <t>Town</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Maximum Validation for Extended</t>
   </si>
   <si>
-    <t>Maximum Validation for self</t>
-  </si>
-  <si>
     <t>Minimum Validation for self</t>
   </si>
   <si>
@@ -345,6 +342,12 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>MaxChild</t>
+  </si>
+  <si>
+    <t>MinChild</t>
   </si>
 </sst>
 </file>
@@ -1459,13 +1462,13 @@
         <v>14</v>
       </c>
       <c r="Q1" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="S1" s="35" t="s">
         <v>87</v>
-      </c>
-      <c r="S1" s="35" t="s">
-        <v>88</v>
       </c>
       <c r="T1" s="35" t="s">
         <v>38</v>
@@ -1497,22 +1500,22 @@
         <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>22</v>
@@ -1521,13 +1524,13 @@
         <v>10000</v>
       </c>
       <c r="Q2" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="R2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>93</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>94</v>
       </c>
       <c r="T2" s="36">
         <v>35919</v>
@@ -2636,7 +2639,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2663,7 +2666,7 @@
         <v>65</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>66</v>
@@ -2701,7 +2704,7 @@
         <v>75</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>76</v>
@@ -2725,7 +2728,7 @@
         <v>75</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>77</v>
@@ -2746,7 +2749,7 @@
         <v>75</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>78</v>
@@ -2767,7 +2770,7 @@
         <v>75</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>79</v>
@@ -2788,10 +2791,10 @@
         <v>75</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -2809,10 +2812,10 @@
         <v>75</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -2830,10 +2833,10 @@
         <v>75</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -2851,10 +2854,10 @@
         <v>75</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>

</xml_diff>

<commit_message>
new tb and excel
</commit_message>
<xml_diff>
--- a/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
+++ b/ILR_TestSuite/New Business/SalesAppBase/TestData.xlsx
@@ -5,26 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992107\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G992127\Documents\GitHub\ILR_TestSuite\ILR_TestSuite\New Business\SalesAppBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD5C1B-D753-4409-A6DB-2C5836D6F59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE000BA-33CB-4E1A-9D0B-2DE0A8A7892D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="9" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="8" xr2:uid="{6BEDAF8A-103E-4980-A29E-F252802A64CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="PolicyHolder_Details" sheetId="1" r:id="rId1"/>
-    <sheet name="CoverAmount" sheetId="16" r:id="rId2"/>
+    <sheet name="CoverAmount" sheetId="16" r:id="rId1"/>
+    <sheet name="PolicyHolder_Details" sheetId="1" r:id="rId2"/>
     <sheet name="CoverDropDown" sheetId="14" r:id="rId3"/>
     <sheet name="Cover_Coordinates" sheetId="13" r:id="rId4"/>
     <sheet name="PLA" sheetId="5" r:id="rId5"/>
     <sheet name="Affordability_Check" sheetId="8" r:id="rId6"/>
     <sheet name="Scenarios" sheetId="17" r:id="rId7"/>
     <sheet name="Extended" sheetId="7" r:id="rId8"/>
-    <sheet name="Parent" sheetId="11" r:id="rId9"/>
+    <sheet name="Parents" sheetId="11" r:id="rId9"/>
     <sheet name="Spouse" sheetId="6" r:id="rId10"/>
     <sheet name="Beneficiaries" sheetId="9" r:id="rId11"/>
-    <sheet name="Child" sheetId="12" r:id="rId12"/>
+    <sheet name="Children" sheetId="12" r:id="rId12"/>
     <sheet name="PolicyPayer" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="95">
   <si>
     <t>Town</t>
   </si>
@@ -181,18 +181,6 @@
   </si>
   <si>
     <t>Account Number</t>
-  </si>
-  <si>
-    <t>PLA1</t>
-  </si>
-  <si>
-    <t>Parent1</t>
-  </si>
-  <si>
-    <t>Child1</t>
-  </si>
-  <si>
-    <t>Child2</t>
   </si>
   <si>
     <t>LindoKuhle</t>
@@ -349,25 +337,13 @@
     <t>MaxMinAgeExtended</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>04/03/2022 11:52:11</t>
-  </si>
-  <si>
-    <t>04/03/2022 11:52:39</t>
-  </si>
-  <si>
-    <t>04/03/2022 11:52:51</t>
-  </si>
-  <si>
-    <t>04/03/2022 11:53:07</t>
-  </si>
-  <si>
-    <t>04/03/2022 11:53:21</t>
+    <t>Scenario_id</t>
+  </si>
+  <si>
+    <t>scenario_id</t>
+  </si>
+  <si>
+    <t>0789654566</t>
   </si>
 </sst>
 </file>
@@ -467,14 +443,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -518,7 +494,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -602,6 +578,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -611,7 +611,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -683,20 +683,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,19 +711,7 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -734,22 +722,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -762,6 +740,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -782,7 +762,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -795,6 +775,8 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1091,8 +1073,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77094FBE-62A7-4D62-9AD5-A2591B43D462}" name="Table2" displayName="Table2" ref="A1:I6" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I6" xr:uid="{77094FBE-62A7-4D62-9AD5-A2591B43D462}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77094FBE-62A7-4D62-9AD5-A2591B43D462}" name="Table2" displayName="Table2" ref="A1:I10" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I10" xr:uid="{77094FBE-62A7-4D62-9AD5-A2591B43D462}"/>
   <tableColumns count="9">
     <tableColumn id="2" xr3:uid="{6F04CA4E-DCDF-4D0E-864E-A4EC9DCC22FA}" name="Product" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{90CFC39C-5F10-4E1C-A1C9-7C8B4689C428}" name="Functionality" dataDxfId="7"/>
@@ -1404,435 +1386,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42906E6D-7A8E-4EC7-BEBD-C72FF8B2CEAE}">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="2">
-        <v>10000</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="R2" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="S2" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="T2" s="30">
-        <v>35919</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{2B0DDEB7-EB30-4148-9844-AB5C379E22BB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44766631-B11A-4479-8024-A9637BA1BEB4}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="9">
-        <v>36202</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99D9670-810C-4DE3-B59B-B8F4007A7BBA}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="7">
-        <v>36202</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G7" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99637A6-F889-4564-89B2-AF62D5E8EE61}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9">
-        <v>36202</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC2C190-2299-448D-81E7-FE582936E6E6}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2">
-        <v>830678899</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="10">
-        <v>62429363625</v>
-      </c>
-      <c r="G2" s="2">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1A9CEFBF-6668-43EE-8C58-295655E6BCFD}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0884330D-945B-460E-9013-EA13CCDB12FF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1847,15 +1400,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>60000</v>
@@ -1863,7 +1416,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>15000</v>
@@ -1871,7 +1424,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>7500</v>
@@ -1879,7 +1432,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>10000</v>
@@ -1887,7 +1440,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>20000</v>
@@ -1916,6 +1469,459 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44766631-B11A-4479-8024-A9637BA1BEB4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9">
+        <v>36202</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99D9670-810C-4DE3-B59B-B8F4007A7BBA}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="7">
+        <v>36202</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99637A6-F889-4564-89B2-AF62D5E8EE61}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9">
+        <v>36202</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="9">
+        <v>36203</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC2C190-2299-448D-81E7-FE582936E6E6}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2">
+        <v>830678899</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="10">
+        <v>62429363625</v>
+      </c>
+      <c r="H2" s="2">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{1A9CEFBF-6668-43EE-8C58-295655E6BCFD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42906E6D-7A8E-4EC7-BEBD-C72FF8B2CEAE}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="U2" s="36">
+        <v>35919</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{2B0DDEB7-EB30-4148-9844-AB5C379E22BB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8655D703-28F5-487A-8779-E3AC589F989A}">
   <dimension ref="A1:C9"/>
@@ -1934,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1945,7 +1951,7 @@
         <v>12.5</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1956,7 +1962,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1967,7 +1973,7 @@
         <v>37.5</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1978,7 +1984,7 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2037,57 +2043,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="36"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2369,7 +2375,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2382,8 +2388,6 @@
     <col min="8" max="8" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -2428,8 +2432,8 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
+      <c r="A2" s="2">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2497,7 +2501,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -2578,11 +2582,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{2ED677DD-E8AF-421A-8C90-EED6078DC1A9}">
-  <dimension ref="A1:M6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED677DD-E8AF-421A-8C90-EED6078DC1A9}">
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2598,216 +2602,201 @@
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:13" x14ac:dyDescent="0.35" outlineLevel="0" r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="H1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="L1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="M1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row spans="1:13" ht="48" x14ac:dyDescent="0.35" outlineLevel="0" r="2">
+    </row>
+    <row r="2" spans="1:13" ht="48" x14ac:dyDescent="0.35">
       <c r="A2" s="24">
         <v>1000</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>96</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="F2" s="27"/>
       <c r="G2" s="27"/>
-      <c r="H2" s="33" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="I2" s="32" t="inlineStr">
-        <is>
-          <t>08/03/2022 18:50:31</t>
-        </is>
-      </c>
-      <c r="K2" s="34">
-        <f>COUNTIF(Table2[Test_Results],"Passed")</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="34">
-        <f>COUNTIF(Table2[Test_Results],"Failed")</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="34">
-        <f>SUM(K2:L2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:13" ht="36" x14ac:dyDescent="0.35" outlineLevel="0" r="3">
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+    </row>
+    <row r="3" spans="1:13" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="24">
         <v>1000</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>96</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F3" s="27"/>
       <c r="G3" s="27"/>
-      <c r="H3" s="33" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I3" s="32" t="inlineStr">
-        <is>
-          <t>08/03/2022 14:45:33</t>
-        </is>
-      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row spans="1:13" ht="24" x14ac:dyDescent="0.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.35">
       <c r="A4" s="24">
         <v>1000</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>96</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F4" s="28"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="33" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I4" s="32" t="inlineStr">
-        <is>
-          <t>08/03/2022 14:45:44</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:13" ht="24" x14ac:dyDescent="0.35" outlineLevel="0" r="5">
+      <c r="H4" s="2"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:13" ht="24" x14ac:dyDescent="0.35">
       <c r="A5" s="24">
         <v>1000</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>96</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F5" s="28"/>
       <c r="G5" s="28"/>
-      <c r="H5" s="31" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I5" s="32" t="inlineStr">
-        <is>
-          <t>08/03/2022 14:46:02</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:13" ht="24" x14ac:dyDescent="0.35" outlineLevel="0" r="6">
+      <c r="H5" s="2"/>
+      <c r="I5" s="30"/>
+    </row>
+    <row r="6" spans="1:13" ht="24" x14ac:dyDescent="0.35">
       <c r="A6" s="24">
         <v>1000</v>
       </c>
       <c r="B6" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>96</v>
-      </c>
+      <c r="F6" s="28"/>
       <c r="G6" s="28"/>
-      <c r="H6" s="33" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="I6" s="32" t="inlineStr">
-        <is>
-          <t>08/03/2022 14:46:14</t>
-        </is>
-      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="24"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -2821,7 +2810,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2853,12 +2842,12 @@
         <v>33</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>45</v>
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
@@ -2875,8 +2864,8 @@
       <c r="F2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>51</v>
+      <c r="G2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2888,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A25D57-60AB-4959-A648-53F314C54D9C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2921,8 +2910,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>46</v>
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>

</xml_diff>